<commit_message>
first minimalistic lobby-stat-site, implementation of controller and service
</commit_message>
<xml_diff>
--- a/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
+++ b/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnerermichael/Desktop/Informatik/4. Semester/PS SoftwareEngineering/Implementierung/g1t1/time-records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01AFEAA-861C-A741-925E-FE776EE3E569}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9786535C-3162-CB4B-8C12-2C4960F850F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Datum</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Statistik-Klasse sowie Bug-fixes bei Round</t>
+  </si>
+  <si>
+    <t>Erste Statistik-Services</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -766,9 +769,18 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7"/>
-      <c r="D16" s="3"/>
+      <c r="A16" s="8">
+        <v>43921</v>
+      </c>
+      <c r="B16" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="8"/>

</xml_diff>

<commit_message>
some more stats and cleaned up directory
</commit_message>
<xml_diff>
--- a/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
+++ b/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnerermichael/Desktop/Informatik/4. Semester/PS SoftwareEngineering/Implementierung/g1t1/time-records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9786535C-3162-CB4B-8C12-2C4960F850F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13674860-9361-9A4A-A670-928B75E2A6EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Datum</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Erste Statistik-Services</t>
+  </si>
+  <si>
+    <t>Erweiterung Statistiken</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -783,9 +786,18 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="8"/>
-      <c r="B17" s="7"/>
-      <c r="D17" s="3"/>
+      <c r="A17" s="8">
+        <v>43922</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="8"/>

</xml_diff>

<commit_message>
Most Successfull player + Vereinheitlichung
</commit_message>
<xml_diff>
--- a/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
+++ b/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnerermichael/Desktop/Informatik/4. Semester/PS SoftwareEngineering/Implementierung/g1t1/time-records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13674860-9361-9A4A-A670-928B75E2A6EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E39C0B-46B6-8E42-A48D-F66B643BA187}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Erweiterung Statistiken</t>
+  </si>
+  <si>
+    <t>Erste Highscore_seite</t>
+  </si>
+  <si>
+    <t>Sechstes Meeting, Statusbesprechung</t>
+  </si>
+  <si>
+    <t>Meeting, Statusbesprechung</t>
+  </si>
+  <si>
+    <t>Meeting, Mergen+Besprechen</t>
+  </si>
+  <si>
+    <t>Mehr Statistik, Vereinheitlichung</t>
   </si>
 </sst>
 </file>
@@ -544,13 +559,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855F84B-A166-7442-8B83-EBB2C6A67214}">
-  <dimension ref="A1:D1001"/>
+  <dimension ref="A1:D1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -773,56 +788,101 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="8">
-        <v>43921</v>
+        <v>43916</v>
       </c>
       <c r="B16" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="8">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B17" s="7">
-        <v>0.10416666666666667</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="8">
+        <v>43922</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="8"/>
-      <c r="B18" s="7"/>
-      <c r="D18" s="3"/>
-    </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="8"/>
-      <c r="B19" s="7"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="8">
+        <v>43922</v>
+      </c>
+      <c r="B19" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="8">
+        <v>43927</v>
+      </c>
+      <c r="B20" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="8">
+        <v>43928</v>
+      </c>
+      <c r="B21" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="8">
+        <v>43930</v>
+      </c>
+      <c r="B22" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="8"/>
@@ -5715,7 +5775,22 @@
       <c r="D1000" s="3"/>
     </row>
     <row r="1001" spans="1:4">
-      <c r="A1001" s="2"/>
+      <c r="A1001" s="8"/>
+      <c r="B1001" s="7"/>
+      <c r="D1001" s="3"/>
+    </row>
+    <row r="1002" spans="1:4">
+      <c r="A1002" s="8"/>
+      <c r="B1002" s="7"/>
+      <c r="D1002" s="3"/>
+    </row>
+    <row r="1003" spans="1:4">
+      <c r="A1003" s="8"/>
+      <c r="B1003" s="7"/>
+      <c r="D1003" s="3"/>
+    </row>
+    <row r="1004" spans="1:4">
+      <c r="A1004" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5727,7 +5802,7 @@
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C9 C10:C1000</xm:sqref>
+          <xm:sqref>C2:C9 C10:C1003</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
a demo for creating new rounds, time-records
</commit_message>
<xml_diff>
--- a/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
+++ b/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnerermichael/Desktop/Informatik/4. Semester/PS SoftwareEngineering/Implementierung/g1t1/time-records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE52E36C-7B0B-9F46-9C32-E66B600880A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772B4C86-D906-0C49-9E3D-C46C0A5743DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Datum</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Meeting, Vorbereitung PS-Stunde</t>
+  </si>
+  <si>
+    <t>Rundenerzeugung, Spiellogik</t>
+  </si>
+  <si>
+    <t>JPA und Hibernate, Websockets</t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -916,14 +922,32 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="8"/>
-      <c r="B25" s="7"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="8">
+        <v>43937</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="8"/>
-      <c r="B26" s="7"/>
-      <c r="D26" s="3"/>
+      <c r="A26" s="8">
+        <v>43937</v>
+      </c>
+      <c r="B26" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="8"/>

</xml_diff>

<commit_message>
new roundchannel in websocketmanager, time-records
</commit_message>
<xml_diff>
--- a/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
+++ b/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnerermichael/Desktop/Informatik/4. Semester/PS SoftwareEngineering/Implementierung/g1t1/time-records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DFE5C7-5079-8A4D-98E7-57E8BC371393}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2E3EB8-A0D2-2C42-9A1E-0F30680FEAFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>Datum</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Roundservice-tests</t>
+  </si>
+  <si>
+    <t>Statusbesprechung</t>
+  </si>
+  <si>
+    <t>Branchchecking</t>
+  </si>
+  <si>
+    <t>Some gamelogik</t>
+  </si>
+  <si>
+    <t>Start round via flip + Demo-GUI</t>
   </si>
 </sst>
 </file>
@@ -580,7 +592,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -996,29 +1008,74 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="8"/>
-      <c r="B30" s="7"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="8">
+        <v>43946</v>
+      </c>
+      <c r="B30" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="8"/>
-      <c r="B31" s="7"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="8">
+        <v>43947</v>
+      </c>
+      <c r="B31" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="8"/>
-      <c r="B32" s="7"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="8">
+        <v>43948</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="8"/>
-      <c r="B33" s="7"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="8">
+        <v>43948</v>
+      </c>
+      <c r="B33" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7"/>
-      <c r="D34" s="3"/>
+      <c r="A34" s="8">
+        <v>43949</v>
+      </c>
+      <c r="B34" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="8"/>

</xml_diff>

<commit_message>
Send new round to players + countdown
</commit_message>
<xml_diff>
--- a/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
+++ b/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnerermichael/Desktop/Informatik/4. Semester/PS SoftwareEngineering/Implementierung/g1t1/time-records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2E3EB8-A0D2-2C42-9A1E-0F30680FEAFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B85BEDF-B819-8B4E-9245-478343EE8A62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>Datum</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Start round via flip + Demo-GUI</t>
+  </si>
+  <si>
+    <t>Update gameRoom</t>
+  </si>
+  <si>
+    <t>Debug-Websockets</t>
+  </si>
+  <si>
+    <t>Websocket, startround+countdown</t>
   </si>
 </sst>
 </file>
@@ -589,10 +598,10 @@
   <dimension ref="A1:D1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
+      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1078,29 +1087,74 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="8"/>
-      <c r="B35" s="7"/>
-      <c r="D35" s="3"/>
+      <c r="A35" s="8">
+        <v>43950</v>
+      </c>
+      <c r="B35" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="8"/>
-      <c r="B36" s="7"/>
-      <c r="D36" s="3"/>
+      <c r="A36" s="8">
+        <v>43952</v>
+      </c>
+      <c r="B36" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
-      <c r="D37" s="3"/>
+      <c r="A37" s="8">
+        <v>43953</v>
+      </c>
+      <c r="B37" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="8">
+        <v>43953</v>
+      </c>
+      <c r="B38" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="8">
+        <v>43954</v>
+      </c>
+      <c r="B39" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="8"/>

</xml_diff>

<commit_message>
Resolve "Start round via flip"
</commit_message>
<xml_diff>
--- a/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
+++ b/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnerermichael/Desktop/Informatik/4. Semester/PS SoftwareEngineering/Implementierung/g1t1/time-records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DFE5C7-5079-8A4D-98E7-57E8BC371393}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B85BEDF-B819-8B4E-9245-478343EE8A62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>Datum</t>
   </si>
@@ -166,6 +166,27 @@
   </si>
   <si>
     <t>Roundservice-tests</t>
+  </si>
+  <si>
+    <t>Statusbesprechung</t>
+  </si>
+  <si>
+    <t>Branchchecking</t>
+  </si>
+  <si>
+    <t>Some gamelogik</t>
+  </si>
+  <si>
+    <t>Start round via flip + Demo-GUI</t>
+  </si>
+  <si>
+    <t>Update gameRoom</t>
+  </si>
+  <si>
+    <t>Debug-Websockets</t>
+  </si>
+  <si>
+    <t>Websocket, startround+countdown</t>
   </si>
 </sst>
 </file>
@@ -577,10 +598,10 @@
   <dimension ref="A1:D1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -996,54 +1017,144 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="8"/>
-      <c r="B30" s="7"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="8">
+        <v>43946</v>
+      </c>
+      <c r="B30" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="8"/>
-      <c r="B31" s="7"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="8">
+        <v>43947</v>
+      </c>
+      <c r="B31" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="8"/>
-      <c r="B32" s="7"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="8">
+        <v>43948</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="8"/>
-      <c r="B33" s="7"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="8">
+        <v>43948</v>
+      </c>
+      <c r="B33" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7"/>
-      <c r="D34" s="3"/>
+      <c r="A34" s="8">
+        <v>43949</v>
+      </c>
+      <c r="B34" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="8"/>
-      <c r="B35" s="7"/>
-      <c r="D35" s="3"/>
+      <c r="A35" s="8">
+        <v>43950</v>
+      </c>
+      <c r="B35" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="8"/>
-      <c r="B36" s="7"/>
-      <c r="D36" s="3"/>
+      <c r="A36" s="8">
+        <v>43952</v>
+      </c>
+      <c r="B36" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7"/>
-      <c r="D37" s="3"/>
+      <c r="A37" s="8">
+        <v>43953</v>
+      </c>
+      <c r="B37" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="8">
+        <v>43953</v>
+      </c>
+      <c r="B38" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="8">
+        <v>43954</v>
+      </c>
+      <c r="B39" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="8"/>

</xml_diff>